<commit_message>
sorted with a,b,c; %.1f for pie charts
</commit_message>
<xml_diff>
--- a/data/data_processed.xlsx
+++ b/data/data_processed.xlsx
@@ -867,17 +867,17 @@
   <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O23" activeCellId="0" sqref="O23"/>
+      <selection pane="topLeft" activeCell="O73" activeCellId="0" sqref="O73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
@@ -966,6 +966,12 @@
       <c r="L2" s="1" t="n">
         <v>16.2695759688477</v>
       </c>
+      <c r="N2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="Q2" s="0" t="n">
         <f aca="false">SUM(N2:N120)</f>
         <v>22302.1391483783</v>
@@ -1012,6 +1018,12 @@
       <c r="L3" s="1" t="n">
         <v>23.0925226479102</v>
       </c>
+      <c r="N3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -1050,6 +1062,12 @@
       <c r="L4" s="1" t="n">
         <v>11.0771278356335</v>
       </c>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -1134,6 +1152,12 @@
       <c r="L6" s="1" t="n">
         <v>70.5003797889186</v>
       </c>
+      <c r="N6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -1356,6 +1380,12 @@
       <c r="L11" s="1" t="n">
         <v>2669.91944946975</v>
       </c>
+      <c r="N11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -1440,6 +1470,12 @@
       <c r="L13" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="N13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -1800,6 +1836,12 @@
       <c r="L21" s="1" t="n">
         <v>771.340861552305</v>
       </c>
+      <c r="N21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -4184,8 +4226,12 @@
       <c r="L73" s="1" t="n">
         <v>36.0723577785088</v>
       </c>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
+      <c r="N73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O73" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">

</xml_diff>